<commit_message>
fix se url tests
</commit_message>
<xml_diff>
--- a/src/test/resources/net/pageseeder/ox/web/mps4/mswSubmission/msw-data-source-spreadsheet-test.xlsx
+++ b/src/test/resources/net/pageseeder/ox/web/mps4/mswSubmission/msw-data-source-spreadsheet-test.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24827"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vku\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\workspace\pbs\berliozweb-mps4-ox-models\src\test\resources\net\pageseeder\ox\web\mps4\mswSubmission\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{043763DB-0FAA-4773-9F1E-E5C41E23849E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66EDD234-54F6-435C-81D5-A103B88D46A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="71">
   <si>
     <t>Meeting last considered at</t>
   </si>
@@ -267,6 +267,15 @@
   </si>
   <si>
     <t>Pending PBAC Outcome</t>
+  </si>
+  <si>
+    <t>step-2-see-url-title</t>
+  </si>
+  <si>
+    <t>http://www.pbs.gov.au/info/industry/listing/elements/pbac-meetings/pbac-consumer-comments</t>
+  </si>
+  <si>
+    <t>PBAC Consumer Comment</t>
   </si>
 </sst>
 </file>
@@ -587,7 +596,35 @@
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="25">
+    <dxf>
+      <font>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -1249,28 +1286,29 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table134" displayName="Table134" ref="B1:T10" totalsRowShown="0" headerRowDxfId="23" dataDxfId="21" headerRowBorderDxfId="22" tableBorderDxfId="20" totalsRowBorderDxfId="19">
-  <autoFilter ref="B1:T10" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
-  <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="case-id" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="meeting-date" dataDxfId="17"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="pbac-outcome-status" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="drug-name" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="brand-names" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="sponsors" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="purpose" dataDxfId="12"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="type-listing" dataDxfId="11"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="submission-type" dataDxfId="10"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="comment" dataDxfId="9"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="resubmission" dataDxfId="8"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="Meeting last considered at" dataDxfId="7"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="related-medicines" dataDxfId="6"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="status" dataDxfId="5"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="step-1-status" dataDxfId="4"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="step-2-status" dataDxfId="3"/>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="step-2-open-date" dataDxfId="2"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="step-2-closed-date" dataDxfId="1"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="step-2-see-url" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table134" displayName="Table134" ref="B1:U10" totalsRowShown="0" headerRowDxfId="24" dataDxfId="22" headerRowBorderDxfId="23" tableBorderDxfId="21" totalsRowBorderDxfId="20">
+  <autoFilter ref="B1:U10" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+  <tableColumns count="20">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="case-id" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="meeting-date" dataDxfId="18"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="pbac-outcome-status" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="drug-name" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="brand-names" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="sponsors" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="purpose" dataDxfId="13"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="type-listing" dataDxfId="12"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="submission-type" dataDxfId="11"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="comment" dataDxfId="10"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="resubmission" dataDxfId="9"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="Meeting last considered at" dataDxfId="8"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="related-medicines" dataDxfId="7"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="status" dataDxfId="6"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="step-1-status" dataDxfId="5"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="step-2-status" dataDxfId="4"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="step-2-open-date" dataDxfId="3"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="step-2-closed-date" dataDxfId="2"/>
+    <tableColumn id="18" xr3:uid="{1F84CD1D-DB39-4D49-87AE-C3093B67AA71}" name="step-2-see-url" dataDxfId="0" dataCellStyle="Explanatory Text"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="step-2-see-url-title" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1597,11 +1635,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:T44"/>
+  <dimension ref="B1:U44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
+      <selection pane="bottomLeft" activeCell="U3" sqref="U3:U10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="60" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1622,12 +1660,13 @@
     <col min="17" max="17" width="18.42578125" style="1" customWidth="1"/>
     <col min="18" max="18" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="24.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.28515625" style="1" customWidth="1"/>
-    <col min="22" max="16384" width="9.28515625" style="1"/>
+    <col min="20" max="20" width="17.28515625" style="1" customWidth="1"/>
+    <col min="21" max="21" width="24.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.28515625" style="1" customWidth="1"/>
+    <col min="23" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:20" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:21" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>46</v>
       </c>
@@ -1685,8 +1724,11 @@
       <c r="T1" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="2" spans="2:20" s="33" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U1" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="2:21" s="33" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="21" t="s">
         <v>37</v>
       </c>
@@ -1731,11 +1773,14 @@
       <c r="S2" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="T2" s="45">
-        <v>4024</v>
-      </c>
-    </row>
-    <row r="3" spans="2:20" s="6" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T2" s="45" t="s">
+        <v>69</v>
+      </c>
+      <c r="U2" s="15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="2:21" s="6" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="21" t="s">
         <v>38</v>
       </c>
@@ -1784,11 +1829,14 @@
       <c r="S3" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="T3" s="45">
-        <v>4024</v>
-      </c>
-    </row>
-    <row r="4" spans="2:20" s="6" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="T3" s="45" t="s">
+        <v>69</v>
+      </c>
+      <c r="U3" s="15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="2:21" s="6" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="B4" s="21" t="s">
         <v>39</v>
       </c>
@@ -1833,11 +1881,14 @@
       <c r="S4" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="T4" s="45">
-        <v>4024</v>
-      </c>
-    </row>
-    <row r="5" spans="2:20" s="6" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T4" s="45" t="s">
+        <v>69</v>
+      </c>
+      <c r="U4" s="15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="2:21" s="6" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="21" t="s">
         <v>40</v>
       </c>
@@ -1882,11 +1933,14 @@
       <c r="S5" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="T5" s="45">
-        <v>4024</v>
-      </c>
-    </row>
-    <row r="6" spans="2:20" s="6" customFormat="1" ht="62.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T5" s="45" t="s">
+        <v>69</v>
+      </c>
+      <c r="U5" s="15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="2:21" s="6" customFormat="1" ht="62.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="21" t="s">
         <v>41</v>
       </c>
@@ -1931,11 +1985,14 @@
       <c r="S6" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="T6" s="45">
-        <v>4024</v>
-      </c>
-    </row>
-    <row r="7" spans="2:20" s="6" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T6" s="45" t="s">
+        <v>69</v>
+      </c>
+      <c r="U6" s="15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="2:21" s="6" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="21" t="s">
         <v>42</v>
       </c>
@@ -1980,11 +2037,14 @@
       <c r="S7" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="T7" s="45">
-        <v>4024</v>
-      </c>
-    </row>
-    <row r="8" spans="2:20" s="6" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T7" s="45" t="s">
+        <v>69</v>
+      </c>
+      <c r="U7" s="15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="2:21" s="6" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="21" t="s">
         <v>43</v>
       </c>
@@ -2033,11 +2093,14 @@
       <c r="S8" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="T8" s="45">
-        <v>4024</v>
-      </c>
-    </row>
-    <row r="9" spans="2:20" s="6" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T8" s="45" t="s">
+        <v>69</v>
+      </c>
+      <c r="U8" s="15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="2:21" s="6" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="21" t="s">
         <v>44</v>
       </c>
@@ -2082,11 +2145,14 @@
       <c r="S9" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="T9" s="45">
-        <v>4024</v>
-      </c>
-    </row>
-    <row r="10" spans="2:20" s="6" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="T9" s="45" t="s">
+        <v>69</v>
+      </c>
+      <c r="U9" s="15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="2:21" s="6" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="B10" s="21" t="s">
         <v>45</v>
       </c>
@@ -2131,11 +2197,14 @@
       <c r="S10" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="T10" s="45">
-        <v>4024</v>
-      </c>
-    </row>
-    <row r="11" spans="2:20" s="6" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T10" s="45" t="s">
+        <v>69</v>
+      </c>
+      <c r="U10" s="15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="2:21" s="6" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -2155,8 +2224,9 @@
       <c r="R11" s="17"/>
       <c r="S11" s="17"/>
       <c r="T11" s="17"/>
-    </row>
-    <row r="12" spans="2:20" s="33" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U11" s="17"/>
+    </row>
+    <row r="12" spans="2:21" s="33" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -2176,8 +2246,9 @@
       <c r="R12" s="17"/>
       <c r="S12" s="17"/>
       <c r="T12" s="17"/>
-    </row>
-    <row r="13" spans="2:20" s="6" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U12" s="17"/>
+    </row>
+    <row r="13" spans="2:21" s="6" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -2197,8 +2268,9 @@
       <c r="R13" s="17"/>
       <c r="S13" s="17"/>
       <c r="T13" s="17"/>
-    </row>
-    <row r="14" spans="2:20" s="33" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U13" s="17"/>
+    </row>
+    <row r="14" spans="2:21" s="33" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -2218,8 +2290,9 @@
       <c r="R14" s="17"/>
       <c r="S14" s="17"/>
       <c r="T14" s="17"/>
-    </row>
-    <row r="15" spans="2:20" s="6" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U14" s="17"/>
+    </row>
+    <row r="15" spans="2:21" s="6" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -2239,8 +2312,9 @@
       <c r="R15" s="1"/>
       <c r="S15" s="1"/>
       <c r="T15" s="1"/>
-    </row>
-    <row r="16" spans="2:20" s="6" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U15" s="1"/>
+    </row>
+    <row r="16" spans="2:21" s="6" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -2260,8 +2334,9 @@
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
       <c r="T16" s="1"/>
-    </row>
-    <row r="17" spans="2:20" s="6" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U16" s="1"/>
+    </row>
+    <row r="17" spans="2:21" s="6" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -2281,8 +2356,9 @@
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
       <c r="T17" s="1"/>
-    </row>
-    <row r="18" spans="2:20" s="6" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U17" s="1"/>
+    </row>
+    <row r="18" spans="2:21" s="6" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -2302,8 +2378,9 @@
       <c r="R18" s="1"/>
       <c r="S18" s="1"/>
       <c r="T18" s="1"/>
-    </row>
-    <row r="19" spans="2:20" s="6" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U18" s="1"/>
+    </row>
+    <row r="19" spans="2:21" s="6" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -2323,8 +2400,9 @@
       <c r="R19" s="1"/>
       <c r="S19" s="1"/>
       <c r="T19" s="1"/>
-    </row>
-    <row r="20" spans="2:20" s="41" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U19" s="1"/>
+    </row>
+    <row r="20" spans="2:21" s="41" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -2344,8 +2422,9 @@
       <c r="R20" s="1"/>
       <c r="S20" s="1"/>
       <c r="T20" s="1"/>
-    </row>
-    <row r="21" spans="2:20" s="33" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U20" s="1"/>
+    </row>
+    <row r="21" spans="2:21" s="33" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -2365,8 +2444,9 @@
       <c r="R21" s="1"/>
       <c r="S21" s="1"/>
       <c r="T21" s="1"/>
-    </row>
-    <row r="22" spans="2:20" s="6" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U21" s="1"/>
+    </row>
+    <row r="22" spans="2:21" s="6" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -2386,8 +2466,9 @@
       <c r="R22" s="1"/>
       <c r="S22" s="1"/>
       <c r="T22" s="1"/>
-    </row>
-    <row r="23" spans="2:20" s="33" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U22" s="1"/>
+    </row>
+    <row r="23" spans="2:21" s="33" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -2407,8 +2488,9 @@
       <c r="R23" s="1"/>
       <c r="S23" s="1"/>
       <c r="T23" s="1"/>
-    </row>
-    <row r="24" spans="2:20" s="6" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U23" s="1"/>
+    </row>
+    <row r="24" spans="2:21" s="6" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -2428,8 +2510,9 @@
       <c r="R24" s="1"/>
       <c r="S24" s="1"/>
       <c r="T24" s="1"/>
-    </row>
-    <row r="25" spans="2:20" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="U24" s="1"/>
+    </row>
+    <row r="25" spans="2:21" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -2449,8 +2532,9 @@
       <c r="R25" s="1"/>
       <c r="S25" s="1"/>
       <c r="T25" s="1"/>
-    </row>
-    <row r="26" spans="2:20" s="6" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U25" s="1"/>
+    </row>
+    <row r="26" spans="2:21" s="6" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
@@ -2470,8 +2554,9 @@
       <c r="R26" s="1"/>
       <c r="S26" s="1"/>
       <c r="T26" s="1"/>
-    </row>
-    <row r="27" spans="2:20" s="40" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U26" s="1"/>
+    </row>
+    <row r="27" spans="2:21" s="40" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -2491,8 +2576,9 @@
       <c r="R27" s="1"/>
       <c r="S27" s="1"/>
       <c r="T27" s="1"/>
-    </row>
-    <row r="28" spans="2:20" s="6" customFormat="1" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U27" s="1"/>
+    </row>
+    <row r="28" spans="2:21" s="6" customFormat="1" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -2512,8 +2598,9 @@
       <c r="R28" s="1"/>
       <c r="S28" s="1"/>
       <c r="T28" s="1"/>
-    </row>
-    <row r="29" spans="2:20" s="6" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U28" s="1"/>
+    </row>
+    <row r="29" spans="2:21" s="6" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
@@ -2533,8 +2620,9 @@
       <c r="R29" s="1"/>
       <c r="S29" s="1"/>
       <c r="T29" s="1"/>
-    </row>
-    <row r="30" spans="2:20" s="6" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U29" s="1"/>
+    </row>
+    <row r="30" spans="2:21" s="6" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
@@ -2554,8 +2642,9 @@
       <c r="R30" s="1"/>
       <c r="S30" s="1"/>
       <c r="T30" s="1"/>
-    </row>
-    <row r="31" spans="2:20" s="6" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U30" s="1"/>
+    </row>
+    <row r="31" spans="2:21" s="6" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
@@ -2575,8 +2664,9 @@
       <c r="R31" s="1"/>
       <c r="S31" s="1"/>
       <c r="T31" s="1"/>
-    </row>
-    <row r="32" spans="2:20" s="6" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U31" s="1"/>
+    </row>
+    <row r="32" spans="2:21" s="6" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
@@ -2596,8 +2686,9 @@
       <c r="R32" s="1"/>
       <c r="S32" s="1"/>
       <c r="T32" s="1"/>
-    </row>
-    <row r="33" spans="2:20" s="6" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U32" s="1"/>
+    </row>
+    <row r="33" spans="2:21" s="6" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
@@ -2617,8 +2708,9 @@
       <c r="R33" s="1"/>
       <c r="S33" s="1"/>
       <c r="T33" s="1"/>
-    </row>
-    <row r="34" spans="2:20" s="6" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U33" s="1"/>
+    </row>
+    <row r="34" spans="2:21" s="6" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
@@ -2638,8 +2730,9 @@
       <c r="R34" s="1"/>
       <c r="S34" s="1"/>
       <c r="T34" s="1"/>
-    </row>
-    <row r="35" spans="2:20" s="6" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U34" s="1"/>
+    </row>
+    <row r="35" spans="2:21" s="6" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
@@ -2659,8 +2752,9 @@
       <c r="R35" s="1"/>
       <c r="S35" s="1"/>
       <c r="T35" s="1"/>
-    </row>
-    <row r="36" spans="2:20" s="6" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U35" s="1"/>
+    </row>
+    <row r="36" spans="2:21" s="6" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
@@ -2680,8 +2774,9 @@
       <c r="R36" s="1"/>
       <c r="S36" s="1"/>
       <c r="T36" s="1"/>
-    </row>
-    <row r="44" spans="2:20" s="39" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U36" s="1"/>
+    </row>
+    <row r="44" spans="2:21" s="39" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
@@ -2701,13 +2796,14 @@
       <c r="R44" s="1"/>
       <c r="S44" s="1"/>
       <c r="T44" s="1"/>
+      <c r="U44" s="1"/>
     </row>
   </sheetData>
   <dataValidations xWindow="1442" yWindow="360" count="2">
     <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Length Exceeded" error="This value must be less than or equal to 400 characters long." promptTitle="Text" prompt="Maximum Length: 400 characters." sqref="F2:F9" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>400</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" error=" " promptTitle="Lookup" prompt="This PBAC Meeting Date (Submission) (Submission) record must already exist in Microsoft Dynamics 365 or in this source file." sqref="S2:S10 C2:D10" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" error=" " promptTitle="Lookup" prompt="This PBAC Meeting Date (Submission) (Submission) record must already exist in Microsoft Dynamics 365 or in this source file." sqref="C2:D10 S2:S10" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>